<commit_message>
Add experience & levelling logic
</commit_message>
<xml_diff>
--- a/math.xlsx
+++ b/math.xlsx
@@ -364,7 +364,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Min</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>(Experience multiplier)</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
   </si>
 </sst>
 </file>
@@ -1016,16 +1022,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
@@ -1040,10 +1040,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1991,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77491008"/>
-        <c:axId val="77491584"/>
+        <c:axId val="83044608"/>
+        <c:axId val="83045760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77491008"/>
+        <c:axId val="83044608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2007,12 +2013,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77491584"/>
+        <c:crossAx val="83045760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77491584"/>
+        <c:axId val="83045760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2024,7 +2030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77491008"/>
+        <c:crossAx val="83044608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2155,10 +2161,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.396336441245893</c:v>
+                  <c:v>18.734993995195193</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.396336441245893</c:v>
+                  <c:v>18.734993995195193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,10 +2176,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.308390039906666</c:v>
+                  <c:v>84.641473586924647</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.308390039906666</c:v>
+                  <c:v>84.641473586924647</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2191,8 +2197,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77494464"/>
-        <c:axId val="77495040"/>
+        <c:axId val="83048640"/>
+        <c:axId val="83049216"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2599,11 +2605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77494464"/>
-        <c:axId val="77495040"/>
+        <c:axId val="83048640"/>
+        <c:axId val="83049216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77494464"/>
+        <c:axId val="83048640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2614,14 +2620,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77495040"/>
+        <c:crossAx val="83049216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77495040"/>
+        <c:axId val="83049216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2633,7 +2639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77494464"/>
+        <c:crossAx val="83048640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2745,10 +2751,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.890193662366794</c:v>
+                  <c:v>10.45761180827895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.890193662366794</c:v>
+                  <c:v>10.45761180827895</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2766,8 +2772,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106251392"/>
-        <c:axId val="106251968"/>
+        <c:axId val="105333888"/>
+        <c:axId val="105334464"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2875,82 +2881,82 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>5000000.030387355</c:v>
+                  <c:v>2500000.0290714656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.025004166668111</c:v>
+                  <c:v>25.025008333332931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.025008333332931</c:v>
+                  <c:v>12.52501666666226</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.69167916666493</c:v>
+                  <c:v>8.3583583333183498</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.52501666666226</c:v>
+                  <c:v>6.2750333332977997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.025020833324666</c:v>
+                  <c:v>5.0250416665972493</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.3583583333183498</c:v>
+                  <c:v>4.1917166665466592</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.1678863094999929</c:v>
+                  <c:v>3.5964869045713472</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2750333332977997</c:v>
+                  <c:v>3.1500666663822283</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5805930555049201</c:v>
+                  <c:v>2.8028527773727889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0250416665972493</c:v>
+                  <c:v>2.5250833327777764</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5705003786954617</c:v>
+                  <c:v>2.2978189386545038</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.1917166665466592</c:v>
+                  <c:v>2.1084333323733446</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8712080126679425</c:v>
+                  <c:v>1.9481852551897236</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5964869045713472</c:v>
+                  <c:v>1.8108309508565337</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.3583958330989567</c:v>
+                  <c:v>1.6917916647917057</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.1500666663822283</c:v>
+                  <c:v>1.5876333310578339</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9662473035803916</c:v>
+                  <c:v>1.4957298992314141</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.8028527773727889</c:v>
+                  <c:v>1.4140388856489907</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.656658113558771</c:v>
+                  <c:v>1.3409478032071189</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5250833327777764</c:v>
+                  <c:v>1.2751666622223905</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4060398803092595</c:v>
+                  <c:v>1.2156511853314051</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2978189386545038</c:v>
+                  <c:v>1.1615469637816869</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1990088759666735</c:v>
+                  <c:v>1.1121481816466945</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.1084333323733446</c:v>
+                  <c:v>1.0668666589870877</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0251041655816087</c:v>
+                  <c:v>1.0252083246532946</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2965,11 +2971,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106251392"/>
-        <c:axId val="106251968"/>
+        <c:axId val="105333888"/>
+        <c:axId val="105334464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106251392"/>
+        <c:axId val="105333888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2980,14 +2986,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106251968"/>
+        <c:crossAx val="105334464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106251968"/>
+        <c:axId val="105334464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -3000,7 +3006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106251392"/>
+        <c:crossAx val="105333888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3037,7 +3043,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8BEFA9B-A9EF-470C-99B1-444DB63A8217}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B8BEFA9B-A9EF-470C-99B1-444DB63A8217}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3411,8 +3417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,10 +3483,10 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="58"/>
+      <c r="I4" s="51"/>
       <c r="M4" s="17" t="s">
         <v>46</v>
       </c>
@@ -3511,18 +3517,18 @@
         <v>7</v>
       </c>
       <c r="M5" s="12">
-        <f>ROUNDDOWN(IF(L5=$F$68,$J$60,IF(L5=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L5=$F$68,$J$62,IF(L5=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="58" t="s">
+      <c r="O5" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="S5" s="58" t="s">
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="S5" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="58"/>
+      <c r="T5" s="51"/>
     </row>
     <row r="6" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -3560,7 +3566,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="12">
-        <f>ROUNDDOWN(IF(L6=$F$68,$J$60,IF(L6=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L6=$F$68,$J$62,IF(L6=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>0</v>
       </c>
       <c r="O6" s="17" t="s">
@@ -3575,7 +3581,7 @@
         <v>57</v>
       </c>
       <c r="T6" s="18">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>61</v>
@@ -3617,7 +3623,7 @@
         <v>2</v>
       </c>
       <c r="M7" s="12">
-        <f>ROUNDDOWN(IF(L7=$F$68,$J$60,IF(L7=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L7=$F$68,$J$62,IF(L7=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>15</v>
       </c>
       <c r="O7" s="17" t="s">
@@ -3625,7 +3631,7 @@
       </c>
       <c r="P7" s="44">
         <f>IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$6))*100</f>
-        <v>0.23934675191678023</v>
+        <v>0.47812063515703107</v>
       </c>
       <c r="Q7" s="45" t="s">
         <v>52</v>
@@ -3676,7 +3682,7 @@
         <v>6</v>
       </c>
       <c r="M8" s="12">
-        <f>ROUNDDOWN(IF(L8=$F$68,$J$60,IF(L8=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L8=$F$68,$J$62,IF(L8=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>5</v>
       </c>
       <c r="O8" s="17" t="s">
@@ -3684,7 +3690,7 @@
       </c>
       <c r="P8" s="46">
         <f>IF(P7=0,100000000,100/P7)</f>
-        <v>417.8038732473359</v>
+        <v>209.15223616557901</v>
       </c>
       <c r="Q8" s="45" t="s">
         <v>53</v>
@@ -3735,7 +3741,7 @@
         <v>4</v>
       </c>
       <c r="M9" s="12">
-        <f>ROUNDDOWN(IF(L9=$F$68,$J$60,IF(L9=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L9=$F$68,$J$62,IF(L9=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="17" t="s">
@@ -3743,7 +3749,7 @@
       </c>
       <c r="P9" s="44">
         <f>P8/20</f>
-        <v>20.890193662366794</v>
+        <v>10.457611808278951</v>
       </c>
       <c r="Q9" s="45" t="s">
         <v>45</v>
@@ -3792,7 +3798,7 @@
         <v>3</v>
       </c>
       <c r="M10" s="12">
-        <f>ROUNDDOWN(IF(L10=$F$68,$J$60,IF(L10=$F$69,$J$61,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
+        <f>ROUNDDOWN(IF(L10=$F$68,$J$62,IF(L10=$F$69,$J$63,0))*IF($F$59&lt;$G$59,0,1-EXP(-($F$59-$G$59)/$T$7))*$T$9,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3867,33 +3873,33 @@
     <row r="43" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L44" s="2"/>
-      <c r="M44" s="55" t="s">
+      <c r="M44" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="N44" s="57"/>
-      <c r="O44" s="55" t="s">
+      <c r="N44" s="55"/>
+      <c r="O44" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="57"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="55"/>
     </row>
     <row r="45" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58" t="s">
+      <c r="C45" s="51"/>
+      <c r="D45" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58" t="s">
+      <c r="E45" s="51"/>
+      <c r="F45" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58" t="s">
+      <c r="G45" s="51"/>
+      <c r="H45" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="58"/>
+      <c r="I45" s="51"/>
       <c r="L45" s="32" t="s">
         <v>14</v>
       </c>
@@ -3912,10 +3918,10 @@
       <c r="Q45" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="S45" s="50" t="s">
+      <c r="S45" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="T45" s="51"/>
+      <c r="T45" s="57"/>
     </row>
     <row r="46" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="19" t="s">
@@ -3942,11 +3948,11 @@
       <c r="I46" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L46" s="59">
+      <c r="L46" s="50">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="M46" s="41">
-        <f>$T$9</f>
+        <f t="shared" ref="M46:M71" si="4">$T$9</f>
         <v>100</v>
       </c>
       <c r="N46" s="41">
@@ -3954,16 +3960,16 @@
         <v>9.9999949998430537E-5</v>
       </c>
       <c r="O46" s="39">
-        <f>1-EXP(-L46/$T$6)</f>
-        <v>9.9999999392252903E-9</v>
+        <f t="shared" ref="O46:O71" si="5">1-EXP(-L46/$T$6)</f>
+        <v>1.9999999767428278E-8</v>
       </c>
       <c r="P46" s="35">
         <f>IF(O46=0,10000000000000,1/O46)</f>
-        <v>100000000.60774711</v>
+        <v>50000000.58142931</v>
       </c>
       <c r="Q46" s="36">
         <f>P46/20</f>
-        <v>5000000.030387355</v>
+        <v>2500000.0290714656</v>
       </c>
       <c r="S46" s="32" t="s">
         <v>14</v>
@@ -3977,66 +3983,66 @@
         <v>7</v>
       </c>
       <c r="B47" s="22">
-        <f t="shared" ref="B47:B53" si="4">$C$2*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="B47:B53" si="6">$C$2*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>0.86602540378443871</v>
       </c>
       <c r="C47" s="22">
-        <f t="shared" ref="C47:C53" si="5">$C$2*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="C47:C53" si="7">$C$2*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>0.49999999999999994</v>
       </c>
       <c r="D47" s="22">
-        <f t="shared" ref="D47:D53" si="6">$C$3*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="D47:D53" si="8">$C$3*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>21.650635094610969</v>
       </c>
       <c r="E47" s="22">
-        <f t="shared" ref="E47:E53" si="7">$C$3*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="E47:E53" si="9">$C$3*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>12.499999999999998</v>
       </c>
       <c r="F47" s="22">
-        <f t="shared" ref="F47:F53" si="8">VLOOKUP($A47,$E$6:$J$11,3,FALSE)*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="F47:F53" si="10">VLOOKUP($A47,$E$6:$J$11,3,FALSE)*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>10.825317547305485</v>
       </c>
       <c r="G47" s="22">
-        <f t="shared" ref="G47:G53" si="9">VLOOKUP($A47,$E$6:$J$11,3,FALSE)*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="G47:G53" si="11">VLOOKUP($A47,$E$6:$J$11,3,FALSE)*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>6.2499999999999991</v>
       </c>
       <c r="H47" s="22">
-        <f t="shared" ref="H47:H53" si="10">VLOOKUP($A47,$E$6:$J$11,6,FALSE)*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="H47:H53" si="12">VLOOKUP($A47,$E$6:$J$11,6,FALSE)*COS(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>0</v>
       </c>
       <c r="I47" s="22">
-        <f t="shared" ref="I47:I53" si="11">VLOOKUP($A47,$E$6:$J$11,6,FALSE)*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
+        <f t="shared" ref="I47:I53" si="13">VLOOKUP($A47,$E$6:$J$11,6,FALSE)*SIN(VLOOKUP($A47,$A$6:$C$11,3,FALSE))</f>
         <v>0</v>
       </c>
       <c r="L47" s="33">
         <v>1</v>
       </c>
       <c r="M47" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N47" s="33">
-        <f>(1-EXP(-L47/$T$7))*$T$9</f>
+        <f t="shared" ref="N46:N71" si="14">(1-EXP(-L47/$T$7))*$T$9</f>
         <v>9.5162581964040491</v>
       </c>
       <c r="O47" s="39">
-        <f>1-EXP(-L47/$T$6)</f>
-        <v>9.9950016662497809E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.998001332666921E-3</v>
       </c>
       <c r="P47" s="35">
-        <f t="shared" ref="P47:P70" si="12">1/O47</f>
-        <v>1000.5000833333622</v>
+        <f t="shared" ref="P47:P70" si="15">1/O47</f>
+        <v>500.50016666665863</v>
       </c>
       <c r="Q47" s="36">
-        <f t="shared" ref="Q47:Q71" si="13">P47/20</f>
-        <v>50.025004166668111</v>
+        <f t="shared" ref="Q47:Q71" si="16">P47/20</f>
+        <v>25.025008333332931</v>
       </c>
       <c r="S47" s="47">
         <v>0</v>
       </c>
       <c r="T47" s="47">
         <f>T48</f>
-        <v>21.308390039906666</v>
+        <v>84.641473586924647</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4044,67 +4050,67 @@
         <v>5</v>
       </c>
       <c r="B48" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="C48" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D48" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.531435568635775E-15</v>
       </c>
       <c r="E48" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="F48" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.1886134118146501E-16</v>
       </c>
       <c r="G48" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="H48" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I48" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L48" s="33">
         <v>2</v>
       </c>
       <c r="M48" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N48" s="33">
-        <f>(1-EXP(-L48/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>18.126924692201818</v>
       </c>
       <c r="O48" s="39">
-        <f>1-EXP(-L48/$T$6)</f>
-        <v>1.998001332666921E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.9920106560085156E-3</v>
       </c>
       <c r="P48" s="35">
-        <f t="shared" si="12"/>
-        <v>500.50016666665863</v>
+        <f t="shared" si="15"/>
+        <v>250.50033333324521</v>
       </c>
       <c r="Q48" s="36">
-        <f t="shared" si="13"/>
-        <v>25.025008333332931</v>
+        <f t="shared" si="16"/>
+        <v>12.52501666666226</v>
       </c>
       <c r="S48" s="35">
-        <f>J57</f>
-        <v>2.396336441245893</v>
+        <f>F59</f>
+        <v>18.734993995195193</v>
       </c>
       <c r="T48" s="35">
         <f>(1-EXP(-S48/$T$7))*$T$9</f>
-        <v>21.308390039906666</v>
+        <v>84.641473586924647</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4112,63 +4118,63 @@
         <v>2</v>
       </c>
       <c r="B49" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.86602540378443871</v>
       </c>
       <c r="C49" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="D49" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-21.650635094610969</v>
       </c>
       <c r="E49" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12.499999999999998</v>
       </c>
       <c r="F49" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-19.48557158514987</v>
       </c>
       <c r="G49" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11.249999999999998</v>
       </c>
       <c r="H49" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-12.99038105676658</v>
       </c>
       <c r="I49" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.4999999999999991</v>
       </c>
       <c r="L49" s="33">
         <v>3</v>
       </c>
       <c r="M49" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N49" s="33">
-        <f>(1-EXP(-L49/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>25.918177931828211</v>
       </c>
       <c r="O49" s="39">
-        <f>1-EXP(-L49/$T$6)</f>
-        <v>2.9955044966269995E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.9820359460647232E-3</v>
       </c>
       <c r="P49" s="35">
-        <f t="shared" si="12"/>
-        <v>333.83358333329858</v>
+        <f t="shared" si="15"/>
+        <v>167.167166666367</v>
       </c>
       <c r="Q49" s="36">
-        <f t="shared" si="13"/>
-        <v>16.69167916666493</v>
+        <f t="shared" si="16"/>
+        <v>8.3583583333183498</v>
       </c>
       <c r="S49" s="37">
         <f>S48</f>
-        <v>2.396336441245893</v>
+        <v>18.734993995195193</v>
       </c>
       <c r="T49" s="37">
         <v>0</v>
@@ -4179,59 +4185,59 @@
         <v>6</v>
       </c>
       <c r="B50" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.8660254037844386</v>
       </c>
       <c r="C50" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.50000000000000011</v>
       </c>
       <c r="D50" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-21.650635094610966</v>
       </c>
       <c r="E50" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-12.500000000000004</v>
       </c>
       <c r="F50" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-10.825317547305483</v>
       </c>
       <c r="G50" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-6.2500000000000018</v>
       </c>
       <c r="H50" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-5.196152422706632</v>
       </c>
       <c r="I50" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-3.0000000000000009</v>
       </c>
       <c r="L50" s="33">
         <v>4</v>
       </c>
       <c r="M50" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N50" s="33">
-        <f>(1-EXP(-L50/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>32.967995396436066</v>
       </c>
       <c r="O50" s="39">
-        <f>1-EXP(-L50/$T$6)</f>
-        <v>3.9920106560085156E-3</v>
+        <f t="shared" si="5"/>
+        <v>7.9680851629393423E-3</v>
       </c>
       <c r="P50" s="35">
-        <f t="shared" si="12"/>
-        <v>250.50033333324521</v>
+        <f t="shared" si="15"/>
+        <v>125.50066666595599</v>
       </c>
       <c r="Q50" s="36">
-        <f t="shared" si="13"/>
-        <v>12.52501666666226</v>
+        <f t="shared" si="16"/>
+        <v>6.2750333332977997</v>
       </c>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
@@ -4241,42 +4247,42 @@
         <v>4</v>
       </c>
       <c r="B51" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.83772268236293E-16</v>
       </c>
       <c r="C51" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="D51" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-4.594306705907325E-15</v>
       </c>
       <c r="E51" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-25</v>
       </c>
       <c r="F51" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.756584023544395E-15</v>
       </c>
       <c r="G51" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-15</v>
       </c>
       <c r="H51" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I51" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L51" s="33">
         <v>5</v>
       </c>
       <c r="M51" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N51" s="33">
@@ -4284,80 +4290,80 @@
         <v>39.346934028736655</v>
       </c>
       <c r="O51" s="39">
-        <f>1-EXP(-L51/$T$6)</f>
-        <v>4.9875208073176802E-3</v>
+        <f t="shared" si="5"/>
+        <v>9.9501662508318933E-3</v>
       </c>
       <c r="P51" s="35">
-        <f t="shared" si="12"/>
-        <v>200.50041666649332</v>
+        <f t="shared" si="15"/>
+        <v>100.50083333194499</v>
       </c>
       <c r="Q51" s="36">
-        <f t="shared" si="13"/>
-        <v>10.025020833324666</v>
-      </c>
-      <c r="S51" s="52" t="s">
+        <f t="shared" si="16"/>
+        <v>5.0250416665972493</v>
+      </c>
+      <c r="S51" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="T51" s="53"/>
+      <c r="T51" s="59"/>
     </row>
     <row r="52" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.86602540378443837</v>
       </c>
       <c r="C52" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.50000000000000044</v>
       </c>
       <c r="D52" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21.650635094610958</v>
       </c>
       <c r="E52" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-12.500000000000011</v>
       </c>
       <c r="F52" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>15.155444566227672</v>
       </c>
       <c r="G52" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-8.7500000000000071</v>
       </c>
       <c r="H52" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I52" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L52" s="33">
         <v>6</v>
       </c>
       <c r="M52" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N52" s="33">
-        <f>(1-EXP(-L52/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>45.118836390597359</v>
       </c>
       <c r="O52" s="39">
-        <f>1-EXP(-L52/$T$6)</f>
-        <v>5.9820359460647232E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.1928287138069482E-2</v>
       </c>
       <c r="P52" s="35">
-        <f t="shared" si="12"/>
-        <v>167.167166666367</v>
+        <f t="shared" si="15"/>
+        <v>83.834333330933191</v>
       </c>
       <c r="Q52" s="36">
-        <f t="shared" si="13"/>
-        <v>8.3583583333183498</v>
+        <f t="shared" si="16"/>
+        <v>4.1917166665466592</v>
       </c>
       <c r="S52" s="48" t="s">
         <v>14</v>
@@ -4371,66 +4377,66 @@
         <v>7</v>
       </c>
       <c r="B53" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.86602540378443871</v>
       </c>
       <c r="C53" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="D53" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21.650635094610969</v>
       </c>
       <c r="E53" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12.499999999999998</v>
       </c>
       <c r="F53" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10.825317547305485</v>
       </c>
       <c r="G53" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.2499999999999991</v>
       </c>
       <c r="H53" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I53" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L53" s="33">
         <v>7</v>
       </c>
       <c r="M53" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N53" s="33">
-        <f>(1-EXP(-L53/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>50.341469620859044</v>
       </c>
       <c r="O53" s="39">
-        <f>1-EXP(-L53/$T$6)</f>
-        <v>6.9755570667648925E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.3902455737138109E-2</v>
       </c>
       <c r="P53" s="35">
-        <f t="shared" si="12"/>
-        <v>143.35772618999985</v>
+        <f t="shared" si="15"/>
+        <v>71.929738091426941</v>
       </c>
       <c r="Q53" s="36">
-        <f t="shared" si="13"/>
-        <v>7.1678863094999929</v>
+        <f t="shared" si="16"/>
+        <v>3.5964869045713472</v>
       </c>
       <c r="S53" s="47">
         <v>0</v>
       </c>
       <c r="T53" s="47">
         <f>T54</f>
-        <v>20.890193662366794</v>
+        <v>10.45761180827895</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4449,24 +4455,24 @@
         <v>8</v>
       </c>
       <c r="M54" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N54" s="33">
-        <f>(1-EXP(-L54/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>55.067103588277845</v>
       </c>
       <c r="O54" s="39">
-        <f>1-EXP(-L54/$T$6)</f>
-        <v>7.9680851629393423E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.5872679944714863E-2</v>
       </c>
       <c r="P54" s="35">
-        <f t="shared" si="12"/>
-        <v>125.50066666595599</v>
+        <f t="shared" si="15"/>
+        <v>63.001333327644566</v>
       </c>
       <c r="Q54" s="36">
-        <f t="shared" si="13"/>
-        <v>6.2750333332977997</v>
+        <f t="shared" si="16"/>
+        <v>3.1500666663822283</v>
       </c>
       <c r="S54" s="35">
         <f>J57</f>
@@ -4474,7 +4480,7 @@
       </c>
       <c r="T54" s="35">
         <f>1/(20*(1-EXP(-S54/$T$6)))</f>
-        <v>20.890193662366794</v>
+        <v>10.45761180827895</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4482,24 +4488,24 @@
         <v>9</v>
       </c>
       <c r="M55" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N55" s="33">
-        <f>(1-EXP(-L55/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>59.343034025940092</v>
       </c>
       <c r="O55" s="39">
-        <f>1-EXP(-L55/$T$6)</f>
-        <v>8.9596212271163544E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.7838967641699233E-2</v>
       </c>
       <c r="P55" s="35">
-        <f t="shared" si="12"/>
-        <v>111.6118611100984</v>
+        <f t="shared" si="15"/>
+        <v>56.057055547455775</v>
       </c>
       <c r="Q55" s="36">
-        <f t="shared" si="13"/>
-        <v>5.5805930555049201</v>
+        <f t="shared" si="16"/>
+        <v>2.8028527773727889</v>
       </c>
       <c r="S55" s="37">
         <f>S54</f>
@@ -4533,28 +4539,28 @@
         <v>10</v>
       </c>
       <c r="M56" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N56" s="33">
-        <f>(1-EXP(-L56/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>63.212055882855765</v>
       </c>
       <c r="O56" s="39">
-        <f>1-EXP(-L56/$T$6)</f>
-        <v>9.9501662508318933E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.9801326693244747E-2</v>
       </c>
       <c r="P56" s="35">
-        <f t="shared" si="12"/>
-        <v>100.50083333194499</v>
+        <f t="shared" si="15"/>
+        <v>50.501666655555532</v>
       </c>
       <c r="Q56" s="36">
-        <f t="shared" si="13"/>
-        <v>5.0250416665972493</v>
+        <f t="shared" si="16"/>
+        <v>2.5250833327777764</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="52" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="24">
@@ -4585,29 +4591,29 @@
         <v>11</v>
       </c>
       <c r="M57" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N57" s="33">
-        <f>(1-EXP(-L57/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>66.712891630192047</v>
       </c>
       <c r="O57" s="39">
-        <f>1-EXP(-L57/$T$6)</f>
-        <v>1.0939721224631271E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.175976494878995E-2</v>
       </c>
       <c r="P57" s="35">
-        <f t="shared" si="12"/>
-        <v>91.410007573909226</v>
+        <f t="shared" si="15"/>
+        <v>45.95637877309008</v>
       </c>
       <c r="Q57" s="36">
-        <f t="shared" si="13"/>
-        <v>4.5705003786954617</v>
+        <f t="shared" si="16"/>
+        <v>2.2978189386545038</v>
       </c>
       <c r="R57" s="2"/>
     </row>
     <row r="58" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
+      <c r="A58" s="52"/>
       <c r="B58" s="24">
         <f>$B$72*VLOOKUP($A57,$A$47:$G$53,4,FALSE)</f>
         <v>108.25317547305485</v>
@@ -4628,38 +4634,38 @@
         <v>3.9244186046511613</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="J58" s="12">
-        <f>VLOOKUP(F68,$A$6:$C$11,2,FALSE)-VLOOKUP(F69,$A$6:$C$11,2,FALSE) + IF(VLOOKUP(F68,$A$6:$C$11,2,FALSE)-VLOOKUP(F69,$A$6:$C$11,2,FALSE)&gt;180,-360,IF(VLOOKUP(F68,$A$6:$C$11,2,FALSE)-VLOOKUP(F69,$A$6:$C$11,2,FALSE)&lt;=-180,360,0))</f>
-        <v>60</v>
+        <f>VLOOKUP(F68,$A$6:$C$11,2,FALSE)</f>
+        <v>210</v>
       </c>
       <c r="L58" s="33">
         <v>12</v>
       </c>
       <c r="M58" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N58" s="33">
-        <f>(1-EXP(-L58/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>69.880578808779774</v>
       </c>
       <c r="O58" s="39">
-        <f>1-EXP(-L58/$T$6)</f>
-        <v>1.1928287138069482E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.3714290242090708E-2</v>
       </c>
       <c r="P58" s="35">
-        <f t="shared" si="12"/>
-        <v>83.834333330933191</v>
+        <f t="shared" si="15"/>
+        <v>42.168666647466893</v>
       </c>
       <c r="Q58" s="36">
-        <f t="shared" si="13"/>
-        <v>4.1917166665466592</v>
+        <f t="shared" si="16"/>
+        <v>2.1084333323733446</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="52" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="24">
@@ -4680,38 +4686,38 @@
         <v>16.3386575539493</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J59" s="24">
-        <f>VLOOKUP(F68,$A$6:$C$11,2,FALSE)-F61 + IF(VLOOKUP(F68,$A$6:$C$11,2,FALSE)-F61&gt;180,-360,IF(VLOOKUP(F68,$A$6:$C$11,2,FALSE)-F61&lt;=-180,360,0))</f>
-        <v>43.897886248013947</v>
+        <v>67</v>
+      </c>
+      <c r="J59" s="12">
+        <f>VLOOKUP(F69,$A$6:$C$11,2,FALSE)</f>
+        <v>150</v>
       </c>
       <c r="L59" s="33">
         <v>13</v>
       </c>
       <c r="M59" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N59" s="33">
-        <f>(1-EXP(-L59/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>72.746820696598746</v>
       </c>
       <c r="O59" s="39">
-        <f>1-EXP(-L59/$T$6)</f>
-        <v>1.2915864979712421E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.5664910391250628E-2</v>
       </c>
       <c r="P59" s="35">
-        <f t="shared" si="12"/>
-        <v>77.424160253358849</v>
+        <f t="shared" si="15"/>
+        <v>38.963705103794474</v>
       </c>
       <c r="Q59" s="36">
-        <f t="shared" si="13"/>
-        <v>3.8712080126679425</v>
+        <f t="shared" si="16"/>
+        <v>1.9481852551897236</v>
       </c>
     </row>
     <row r="60" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
+      <c r="A60" s="52"/>
       <c r="B60" s="24">
         <f>$B$72*VLOOKUP($A59,$A$47:$G$53,4,FALSE)</f>
         <v>7.6571778431788751E-15</v>
@@ -4732,38 +4738,38 @@
         <v>2.8990287794943082</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="J60" s="12">
-        <f>1-J59/J58</f>
-        <v>0.26836856253310093</v>
+        <f>J58-J59 + IF(J58-J59&gt;180,-360,IF(J58-J59&lt;=-180,360,0))</f>
+        <v>60</v>
       </c>
       <c r="L60" s="33">
         <v>14</v>
       </c>
       <c r="M60" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N60" s="33">
-        <f>(1-EXP(-L60/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>75.340303605839352</v>
       </c>
       <c r="O60" s="39">
-        <f>1-EXP(-L60/$T$6)</f>
-        <v>1.3902455737138109E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.7611633198753149E-2</v>
       </c>
       <c r="P60" s="35">
-        <f t="shared" si="12"/>
-        <v>71.929738091426941</v>
+        <f t="shared" si="15"/>
+        <v>36.216619017130675</v>
       </c>
       <c r="Q60" s="36">
-        <f t="shared" si="13"/>
-        <v>3.5964869045713472</v>
+        <f t="shared" si="16"/>
+        <v>1.8108309508565337</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="52" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="24">
@@ -4784,38 +4790,38 @@
         <v>166.10211375198605</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="J61" s="12">
-        <f>1-J60</f>
-        <v>0.73163143746689907</v>
+        <v>24</v>
+      </c>
+      <c r="J61" s="24">
+        <f>J58-F61 + IF(J58-F61&gt;180,-360,IF(J58-F61&lt;=-180,360,0))</f>
+        <v>43.897886248013947</v>
       </c>
       <c r="L61" s="33">
         <v>15</v>
       </c>
       <c r="M61" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N61" s="33">
-        <f>(1-EXP(-L61/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>77.686983985157028</v>
       </c>
       <c r="O61" s="39">
-        <f>1-EXP(-L61/$T$6)</f>
-        <v>1.4888060396937353E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.9554466451491845E-2</v>
       </c>
       <c r="P61" s="35">
-        <f t="shared" si="12"/>
-        <v>67.167916661979135</v>
+        <f t="shared" si="15"/>
+        <v>33.835833295834114</v>
       </c>
       <c r="Q61" s="36">
-        <f t="shared" si="13"/>
-        <v>3.3583958330989567</v>
+        <f t="shared" si="16"/>
+        <v>1.6917916647917057</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
+      <c r="A62" s="52"/>
       <c r="B62" s="24">
         <f>$B$72*VLOOKUP($A61,$A$47:$G$53,4,FALSE)</f>
         <v>-108.25317547305485</v>
@@ -4828,39 +4834,46 @@
         <v>7</v>
       </c>
       <c r="F62" s="31" t="b">
-        <f t="shared" ref="F62:F67" si="14">OR(F$61&lt;=VLOOKUP($E62,$A$6:$C$11,2,FALSE),F$61&gt;MAX($B$6:$B$11))</f>
+        <f t="shared" ref="F62:F67" si="17">OR(F$61&lt;=VLOOKUP($E62,$A$6:$C$11,2,FALSE),F$61&gt;MAX($B$6:$B$11))</f>
         <v>0</v>
       </c>
       <c r="G62" s="31" t="b">
-        <f t="shared" ref="G62:G67" si="15">OR(G$61&lt;=VLOOKUP($E62,$A$6:$C$11,2,FALSE),$G$61&gt;MAX($B$6:$B$11))</f>
+        <f t="shared" ref="G62:G67" si="18">OR(G$61&lt;=VLOOKUP($E62,$A$6:$C$11,2,FALSE),$G$61&gt;MAX($B$6:$B$11))</f>
         <v>0</v>
+      </c>
+      <c r="I62" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J62" s="12">
+        <f>1-J61/J60</f>
+        <v>0.26836856253310093</v>
       </c>
       <c r="L62" s="33">
         <v>16</v>
       </c>
       <c r="M62" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N62" s="33">
-        <f>(1-EXP(-L62/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>79.810348200534463</v>
       </c>
       <c r="O62" s="39">
-        <f>1-EXP(-L62/$T$6)</f>
-        <v>1.5872679944714863E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.1493417920802402E-2</v>
       </c>
       <c r="P62" s="35">
-        <f t="shared" si="12"/>
-        <v>63.001333327644566</v>
+        <f t="shared" si="15"/>
+        <v>31.752666621156678</v>
       </c>
       <c r="Q62" s="36">
-        <f t="shared" si="13"/>
-        <v>3.1500666663822283</v>
+        <f t="shared" si="16"/>
+        <v>1.5876333310578339</v>
       </c>
     </row>
     <row r="63" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="54" t="s">
+      <c r="A63" s="52" t="s">
         <v>6</v>
       </c>
       <c r="B63" s="24">
@@ -4873,40 +4886,47 @@
         <v>5</v>
       </c>
       <c r="F63" s="31" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G63" s="31" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J63" s="12">
+        <f>1-J62</f>
+        <v>0.73163143746689907</v>
       </c>
       <c r="L63" s="33">
         <v>17</v>
       </c>
       <c r="M63" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N63" s="33">
-        <f>(1-EXP(-L63/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>81.731647594726525</v>
       </c>
       <c r="O63" s="39">
-        <f>1-EXP(-L63/$T$6)</f>
-        <v>1.6856315365090357E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.3428495362493371E-2</v>
       </c>
       <c r="P63" s="35">
-        <f t="shared" si="12"/>
-        <v>59.324946071607833</v>
+        <f t="shared" si="15"/>
+        <v>29.91459798462828</v>
       </c>
       <c r="Q63" s="36">
-        <f t="shared" si="13"/>
-        <v>2.9662473035803916</v>
+        <f t="shared" si="16"/>
+        <v>1.4957298992314141</v>
       </c>
       <c r="X63"/>
     </row>
     <row r="64" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="54"/>
+      <c r="A64" s="52"/>
       <c r="B64" s="24">
         <f>$B$72*VLOOKUP($A63,$A$47:$G$53,4,FALSE)</f>
         <v>-108.25317547305482</v>
@@ -4919,11 +4939,11 @@
         <v>2</v>
       </c>
       <c r="F64" s="31" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G64" s="31" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I64" s="2"/>
@@ -4932,29 +4952,29 @@
         <v>18</v>
       </c>
       <c r="M64" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N64" s="33">
-        <f>(1-EXP(-L64/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>83.470111177841346</v>
       </c>
       <c r="O64" s="39">
-        <f>1-EXP(-L64/$T$6)</f>
-        <v>1.7838967641699233E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.5359706516876921E-2</v>
       </c>
       <c r="P64" s="35">
-        <f t="shared" si="12"/>
-        <v>56.057055547455775</v>
+        <f t="shared" si="15"/>
+        <v>28.280777712979816</v>
       </c>
       <c r="Q64" s="36">
-        <f t="shared" si="13"/>
-        <v>2.8028527773727889</v>
+        <f t="shared" si="16"/>
+        <v>1.4140388856489907</v>
       </c>
       <c r="X64"/>
     </row>
     <row r="65" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="54" t="s">
+      <c r="A65" s="52" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="24">
@@ -4967,11 +4987,11 @@
         <v>6</v>
       </c>
       <c r="F65" s="31" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="G65" s="31" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="I65" s="2"/>
@@ -4980,29 +5000,29 @@
         <v>19</v>
       </c>
       <c r="M65" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N65" s="33">
-        <f>(1-EXP(-L65/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>85.043138077736486</v>
       </c>
       <c r="O65" s="39">
-        <f>1-EXP(-L65/$T$6)</f>
-        <v>1.8820637757194003E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.728705910880048E-2</v>
       </c>
       <c r="P65" s="35">
-        <f t="shared" si="12"/>
-        <v>53.133162271175422</v>
+        <f t="shared" si="15"/>
+        <v>26.81895606414238</v>
       </c>
       <c r="Q65" s="36">
-        <f t="shared" si="13"/>
-        <v>2.656658113558771</v>
+        <f t="shared" si="16"/>
+        <v>1.3409478032071189</v>
       </c>
       <c r="X65"/>
     </row>
     <row r="66" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
+      <c r="A66" s="52"/>
       <c r="B66" s="24">
         <f>$B$72*VLOOKUP($A65,$A$47:$G$53,4,FALSE)</f>
         <v>-2.2971533529536625E-14</v>
@@ -5015,11 +5035,11 @@
         <v>4</v>
       </c>
       <c r="F66" s="31" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="G66" s="31" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="I66" s="2"/>
@@ -5028,29 +5048,29 @@
         <v>20</v>
       </c>
       <c r="M66" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N66" s="33">
-        <f>(1-EXP(-L66/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>86.466471676338728</v>
       </c>
       <c r="O66" s="39">
-        <f>1-EXP(-L66/$T$6)</f>
-        <v>1.9801326693244747E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.9210560847676823E-2</v>
       </c>
       <c r="P66" s="35">
-        <f t="shared" si="12"/>
-        <v>50.501666655555532</v>
+        <f t="shared" si="15"/>
+        <v>25.503333244447809</v>
       </c>
       <c r="Q66" s="36">
-        <f t="shared" si="13"/>
-        <v>2.5250833327777764</v>
+        <f t="shared" si="16"/>
+        <v>1.2751666622223905</v>
       </c>
       <c r="X66"/>
     </row>
     <row r="67" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="52" t="s">
         <v>3</v>
       </c>
       <c r="B67" s="24">
@@ -5063,11 +5083,11 @@
         <v>3</v>
       </c>
       <c r="F67" s="31" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="G67" s="31" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="I67" s="2"/>
@@ -5076,29 +5096,29 @@
         <v>21</v>
       </c>
       <c r="M67" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N67" s="33">
-        <f>(1-EXP(-L67/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>87.754357174701809</v>
       </c>
       <c r="O67" s="39">
-        <f>1-EXP(-L67/$T$6)</f>
-        <v>2.078103543054044E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.1130219427515491E-2</v>
       </c>
       <c r="P67" s="35">
-        <f t="shared" si="12"/>
-        <v>48.120797606185192</v>
+        <f t="shared" si="15"/>
+        <v>24.313023706628105</v>
       </c>
       <c r="Q67" s="36">
-        <f t="shared" si="13"/>
-        <v>2.4060398803092595</v>
+        <f t="shared" si="16"/>
+        <v>1.2156511853314051</v>
       </c>
       <c r="X67"/>
     </row>
     <row r="68" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="54"/>
+      <c r="A68" s="52"/>
       <c r="B68" s="24">
         <f>$B$72*VLOOKUP($A67,$A$47:$G$53,4,FALSE)</f>
         <v>108.2531754730548</v>
@@ -5124,29 +5144,29 @@
         <v>22</v>
       </c>
       <c r="M68" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N68" s="33">
-        <f>(1-EXP(-L68/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>88.919684163766604</v>
       </c>
       <c r="O68" s="39">
-        <f>1-EXP(-L68/$T$6)</f>
-        <v>2.175976494878995E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.3046042526953321E-2</v>
       </c>
       <c r="P68" s="35">
-        <f t="shared" si="12"/>
-        <v>45.95637877309008</v>
+        <f t="shared" si="15"/>
+        <v>23.230939275633737</v>
       </c>
       <c r="Q68" s="36">
-        <f t="shared" si="13"/>
-        <v>2.2978189386545038</v>
+        <f t="shared" si="16"/>
+        <v>1.1615469637816869</v>
       </c>
       <c r="X68"/>
     </row>
     <row r="69" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="54" t="s">
+      <c r="A69" s="52" t="s">
         <v>27</v>
       </c>
       <c r="B69" s="24">
@@ -5172,28 +5192,28 @@
         <v>23</v>
       </c>
       <c r="M69" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N69" s="33">
-        <f>(1-EXP(-L69/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>89.974115627719613</v>
       </c>
       <c r="O69" s="39">
-        <f>1-EXP(-L69/$T$6)</f>
-        <v>2.2737516226722931E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.4958037809285312E-2</v>
       </c>
       <c r="P69" s="35">
-        <f t="shared" si="12"/>
-        <v>43.980177519333473</v>
+        <f t="shared" si="15"/>
+        <v>22.24296363293389</v>
       </c>
       <c r="Q69" s="36">
-        <f t="shared" si="13"/>
-        <v>2.1990088759666735</v>
+        <f t="shared" si="16"/>
+        <v>1.1121481816466945</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="54"/>
+      <c r="A70" s="52"/>
       <c r="B70" s="24">
         <f>$B$72*F57</f>
         <v>-90.93266739736606</v>
@@ -5217,24 +5237,24 @@
         <v>24</v>
       </c>
       <c r="M70" s="33">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N70" s="33">
-        <f>(1-EXP(-L70/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>90.928204671058751</v>
       </c>
       <c r="O70" s="39">
-        <f>1-EXP(-L70/$T$6)</f>
-        <v>2.3714290242090708E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.6866212922495265E-2</v>
       </c>
       <c r="P70" s="35">
-        <f t="shared" si="12"/>
-        <v>42.168666647466893</v>
+        <f t="shared" si="15"/>
+        <v>21.337333179741755</v>
       </c>
       <c r="Q70" s="36">
-        <f t="shared" si="13"/>
-        <v>2.1084333323733446</v>
+        <f t="shared" si="16"/>
+        <v>1.0668666589870877</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5253,24 +5273,24 @@
         <v>25</v>
       </c>
       <c r="M71" s="34">
-        <f>$T$9</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N71" s="34">
-        <f>(1-EXP(-L71/$T$7))*$T$9</f>
+        <f t="shared" si="14"/>
         <v>91.791500137610115</v>
       </c>
       <c r="O71" s="40">
-        <f>1-EXP(-L71/$T$6)</f>
-        <v>2.4690087971667385E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.8770575499285984E-2</v>
       </c>
       <c r="P71" s="37">
         <f>1/O71</f>
-        <v>40.502083311632177</v>
+        <v>20.504166493065892</v>
       </c>
       <c r="Q71" s="38">
-        <f t="shared" si="13"/>
-        <v>2.0251041655816087</v>
+        <f t="shared" si="16"/>
+        <v>1.0252083246532946</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5348,17 +5368,17 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="O44:Q44"/>
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="S45:T45"/>

</xml_diff>